<commit_message>
Se corrige información del archivo .xlsx
</commit_message>
<xml_diff>
--- a/backend/datos.XLSX
+++ b/backend/datos.XLSX
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos\Actividad_Lectura_de_productos\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B134122-0E74-4270-8282-F44CADA7B759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A662138C-A14C-41D3-AD4D-AB805FA1B87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="productos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Pan</t>
+  </si>
+  <si>
+    <t>Manzanas</t>
+  </si>
+  <si>
+    <t>Pimienta</t>
   </si>
 </sst>
 </file>
@@ -360,13 +366,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -408,6 +417,34 @@
       </c>
       <c r="D3">
         <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>13000</v>
+      </c>
+      <c r="D4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>5000</v>
+      </c>
+      <c r="D5">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se corrige formato de celda en el archivo excel
</commit_message>
<xml_diff>
--- a/backend/datos.XLSX
+++ b/backend/datos.XLSX
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos\Actividad_Lectura_de_productos\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A662138C-A14C-41D3-AD4D-AB805FA1B87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FE197A-B28A-49F5-BC3B-511346239B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,7 +370,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,7 +379,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -392,7 +393,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -406,7 +407,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>20</v>
       </c>
       <c r="B3" t="s">
@@ -420,7 +421,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>30</v>
       </c>
       <c r="B4" t="s">
@@ -434,7 +435,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>40</v>
       </c>
       <c r="B5" t="s">

</xml_diff>

<commit_message>
Se añade función de crear y eliminar productor
</commit_message>
<xml_diff>
--- a/backend/datos.XLSX
+++ b/backend/datos.XLSX
@@ -1,72 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyectos\Actividad_Lectura_de_productos\backend\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FE197A-B28A-49F5-BC3B-511346239B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="productos" sheetId="1" r:id="rId1"/>
+    <sheet name="productos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Precio</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
-    <t>Galletas</t>
-  </si>
-  <si>
-    <t>Pan</t>
-  </si>
-  <si>
-    <t>Manzanas</t>
-  </si>
-  <si>
-    <t>Pimienta</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -366,85 +386,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="A1" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col width="11.28515625" customWidth="1" style="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Precio</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Cantidad</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2">
+      <c r="A2" t="n">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Galletas</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>8000</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3">
+      <c r="A3" t="n">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Pan</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>700</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" t="n">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Manzanas</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>13000</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5">
+      <c r="A5" t="n">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pimienta</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
         <v>5000</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrega función de actualizar productos
</commit_message>
<xml_diff>
--- a/backend/datos.XLSX
+++ b/backend/datos.XLSX
@@ -478,14 +478,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Pimienta</t>
+          <t>Mayonesa</t>
         </is>
       </c>
       <c r="C5" t="n">
         <v>5000</v>
       </c>
       <c r="D5" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merge en la rama main
</commit_message>
<xml_diff>
--- a/backend/datos.XLSX
+++ b/backend/datos.XLSX
@@ -391,7 +391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1:A5"/>
@@ -488,6 +488,22 @@
         <v>100</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Solomito_Carne</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>